<commit_message>
Added new scenarios and test data, and updated SHAFT_Engine
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/certification/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/certification/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -137,12 +137,18 @@
     <t xml:space="preserve">DataSourceType</t>
   </si>
   <si>
+    <t xml:space="preserve">Oracle</t>
+  </si>
+  <si>
     <t xml:space="preserve">MySQL</t>
   </si>
   <si>
     <t xml:space="preserve">DataSourceUsername</t>
   </si>
   <si>
+    <t xml:space="preserve">salesdb</t>
+  </si>
+  <si>
     <t xml:space="preserve">root</t>
   </si>
   <si>
@@ -158,6 +164,9 @@
     <t xml:space="preserve">DataSourceConnectionString</t>
   </si>
   <si>
+    <t xml:space="preserve">jdbc:oracle:thin:@qa.incorta.com:1521:xe</t>
+  </si>
+  <si>
     <t xml:space="preserve">jdbc:mysql://qa.incorta.com:3306/salesdb</t>
   </si>
   <si>
@@ -180,6 +189,24 @@
   </si>
   <si>
     <t xml:space="preserve">File uploaded successfully!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataFileLoadFilter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIRST_NAME="David"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC011 - Add DataSource to Schema using Wizard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DatabaseName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DatabaseTableName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sales</t>
   </si>
   <si>
     <t xml:space="preserve">Supported Browser Types</t>
@@ -413,17 +440,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ30"/>
+  <dimension ref="A1:AMJ34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8:B9"/>
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.53"/>
   </cols>
   <sheetData>
@@ -437,6 +464,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="AMB1" s="0"/>
       <c r="AMC1" s="0"/>
       <c r="AMD1" s="0"/>
       <c r="AME1" s="0"/>
@@ -452,6 +480,7 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
+      <c r="AMB2" s="0"/>
       <c r="AMC2" s="0"/>
       <c r="AMD2" s="0"/>
       <c r="AME2" s="0"/>
@@ -468,6 +497,7 @@
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="AMB3" s="0"/>
       <c r="AMC3" s="0"/>
       <c r="AMD3" s="0"/>
       <c r="AME3" s="0"/>
@@ -484,6 +514,7 @@
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="AMB4" s="0"/>
       <c r="AMC4" s="0"/>
       <c r="AMD4" s="0"/>
       <c r="AME4" s="0"/>
@@ -500,6 +531,7 @@
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="AMB5" s="0"/>
       <c r="AMC5" s="0"/>
       <c r="AMD5" s="0"/>
       <c r="AME5" s="0"/>
@@ -516,6 +548,7 @@
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="AMB6" s="0"/>
       <c r="AMC6" s="0"/>
       <c r="AMD6" s="0"/>
       <c r="AME6" s="0"/>
@@ -532,6 +565,7 @@
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="AMB7" s="0"/>
       <c r="AMC7" s="0"/>
       <c r="AMD7" s="0"/>
       <c r="AME7" s="0"/>
@@ -548,6 +582,7 @@
       <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="AMB8" s="0"/>
       <c r="AMC8" s="0"/>
       <c r="AMD8" s="0"/>
       <c r="AME8" s="0"/>
@@ -564,6 +599,7 @@
       <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="AMB9" s="0"/>
       <c r="AMC9" s="0"/>
       <c r="AMD9" s="0"/>
       <c r="AME9" s="0"/>
@@ -579,6 +615,7 @@
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
+      <c r="AMB10" s="0"/>
       <c r="AMC10" s="0"/>
       <c r="AMD10" s="0"/>
       <c r="AME10" s="0"/>
@@ -596,6 +633,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="6"/>
+      <c r="AMB11" s="0"/>
       <c r="AMC11" s="0"/>
       <c r="AMD11" s="0"/>
       <c r="AME11" s="0"/>
@@ -613,6 +651,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="6"/>
+      <c r="AMB12" s="0"/>
       <c r="AMC12" s="0"/>
       <c r="AMD12" s="0"/>
       <c r="AME12" s="0"/>
@@ -630,6 +669,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="6"/>
+      <c r="AMB13" s="0"/>
       <c r="AMC13" s="0"/>
       <c r="AMD13" s="0"/>
       <c r="AME13" s="0"/>
@@ -645,6 +685,7 @@
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
+      <c r="AMB14" s="0"/>
       <c r="AMC14" s="0"/>
       <c r="AMD14" s="0"/>
       <c r="AME14" s="0"/>
@@ -661,6 +702,7 @@
       <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="AMB15" s="0"/>
       <c r="AMC15" s="0"/>
       <c r="AMD15" s="0"/>
       <c r="AME15" s="0"/>
@@ -676,6 +718,7 @@
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
+      <c r="AMB16" s="0"/>
       <c r="AMC16" s="0"/>
       <c r="AMD16" s="0"/>
       <c r="AME16" s="0"/>
@@ -702,6 +745,7 @@
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
+      <c r="AMB18" s="0"/>
       <c r="AMC18" s="0"/>
       <c r="AMD18" s="0"/>
       <c r="AME18" s="0"/>
@@ -733,6 +777,7 @@
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
+      <c r="AMB21" s="0"/>
       <c r="AMC21" s="0"/>
       <c r="AMD21" s="0"/>
       <c r="AME21" s="0"/>
@@ -746,48 +791,64 @@
       <c r="A22" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="0" t="s">
         <v>38</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="0" t="s">
-        <v>42</v>
+      <c r="C24" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="C25" s="0" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="27" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
+      <c r="AMB27" s="0"/>
       <c r="AMC27" s="0"/>
       <c r="AMD27" s="0"/>
       <c r="AME27" s="0"/>
@@ -799,30 +860,76 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="AMB32" s="0"/>
+      <c r="AMC32" s="0"/>
+      <c r="AMD32" s="0"/>
+      <c r="AME32" s="0"/>
+      <c r="AMF32" s="0"/>
+      <c r="AMG32" s="0"/>
+      <c r="AMH32" s="0"/>
+      <c r="AMI32" s="0"/>
+      <c r="AMJ32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A14:C14"/>
@@ -830,6 +937,7 @@
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A32:C32"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -849,7 +957,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="A8:B9 A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -860,27 +968,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalizing the certification path
. Added new POMs and new test cases
. Modified the test data file to add new parameters
. Updated SHAFT_Engine with some fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/certification/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/certification/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="88">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -77,6 +77,18 @@
     <t xml:space="preserve">schemas/schema-list</t>
   </si>
   <si>
+    <t xml:space="preserve">URL_scheduler_schemas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schedulers/scheduler-schemas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL_scheduler_dashboards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schedulers/scheduler-dashboards</t>
+  </si>
+  <si>
     <t xml:space="preserve">User Credentials</t>
   </si>
   <si>
@@ -207,6 +219,57 @@
   </si>
   <si>
     <t xml:space="preserve">sales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC015 - Schedule Schema Incremental load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SchemaLoadJobDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SchemaLoadJobType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incremental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SchemaLoadJobDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/20/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SchemaLoadJobTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:41 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SchemaLoadJobTimeZone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMT+02:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SchemaLoadJobRecurrence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Recurrence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC016 - Send Dashboard via email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EmailFormat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EmailAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mohab.Mohie@incorta.com</t>
   </si>
   <si>
     <t xml:space="preserve">Supported Browser Types</t>
@@ -232,7 +295,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -264,8 +327,16 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -300,7 +371,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -324,25 +395,36 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -350,18 +432,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -440,505 +519,623 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ34"/>
+  <dimension ref="A1:AMJ46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="64.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AMB1" s="0"/>
-      <c r="AMC1" s="0"/>
-      <c r="AMD1" s="0"/>
-      <c r="AME1" s="0"/>
-      <c r="AMF1" s="0"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="AMB1" s="3"/>
+      <c r="AMC1" s="3"/>
+      <c r="AMD1" s="3"/>
+      <c r="AME1" s="3"/>
+      <c r="AMF1" s="3"/>
+      <c r="AMG1" s="3"/>
+      <c r="AMH1" s="3"/>
+      <c r="AMI1" s="3"/>
+      <c r="AMJ1" s="3"/>
+    </row>
+    <row r="2" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="AMB2" s="0"/>
-      <c r="AMC2" s="0"/>
-      <c r="AMD2" s="0"/>
-      <c r="AME2" s="0"/>
-      <c r="AMF2" s="0"/>
-      <c r="AMG2" s="0"/>
-      <c r="AMH2" s="0"/>
-      <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
-    </row>
-    <row r="3" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="AMB2" s="1"/>
+      <c r="AMC2" s="1"/>
+      <c r="AMD2" s="1"/>
+      <c r="AME2" s="1"/>
+      <c r="AMF2" s="1"/>
+      <c r="AMG2" s="1"/>
+      <c r="AMH2" s="1"/>
+      <c r="AMI2" s="1"/>
+      <c r="AMJ2" s="1"/>
+    </row>
+    <row r="3" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="AMB3" s="0"/>
-      <c r="AMC3" s="0"/>
-      <c r="AMD3" s="0"/>
-      <c r="AME3" s="0"/>
-      <c r="AMF3" s="0"/>
-      <c r="AMG3" s="0"/>
-      <c r="AMH3" s="0"/>
-      <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
-    </row>
-    <row r="4" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="AMB3" s="1"/>
+      <c r="AMC3" s="1"/>
+      <c r="AMD3" s="1"/>
+      <c r="AME3" s="1"/>
+      <c r="AMF3" s="1"/>
+      <c r="AMG3" s="1"/>
+      <c r="AMH3" s="1"/>
+      <c r="AMI3" s="1"/>
+      <c r="AMJ3" s="1"/>
+    </row>
+    <row r="4" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AMB4" s="0"/>
-      <c r="AMC4" s="0"/>
-      <c r="AMD4" s="0"/>
-      <c r="AME4" s="0"/>
-      <c r="AMF4" s="0"/>
-      <c r="AMG4" s="0"/>
-      <c r="AMH4" s="0"/>
-      <c r="AMI4" s="0"/>
-      <c r="AMJ4" s="0"/>
-    </row>
-    <row r="5" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="AMB4" s="1"/>
+      <c r="AMC4" s="1"/>
+      <c r="AMD4" s="1"/>
+      <c r="AME4" s="1"/>
+      <c r="AMF4" s="1"/>
+      <c r="AMG4" s="1"/>
+      <c r="AMH4" s="1"/>
+      <c r="AMI4" s="1"/>
+      <c r="AMJ4" s="1"/>
+    </row>
+    <row r="5" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AMB5" s="0"/>
-      <c r="AMC5" s="0"/>
-      <c r="AMD5" s="0"/>
-      <c r="AME5" s="0"/>
-      <c r="AMF5" s="0"/>
-      <c r="AMG5" s="0"/>
-      <c r="AMH5" s="0"/>
-      <c r="AMI5" s="0"/>
-      <c r="AMJ5" s="0"/>
-    </row>
-    <row r="6" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="AMB5" s="1"/>
+      <c r="AMC5" s="1"/>
+      <c r="AMD5" s="1"/>
+      <c r="AME5" s="1"/>
+      <c r="AMF5" s="1"/>
+      <c r="AMG5" s="1"/>
+      <c r="AMH5" s="1"/>
+      <c r="AMI5" s="1"/>
+      <c r="AMJ5" s="1"/>
+    </row>
+    <row r="6" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="AMB6" s="0"/>
-      <c r="AMC6" s="0"/>
-      <c r="AMD6" s="0"/>
-      <c r="AME6" s="0"/>
-      <c r="AMF6" s="0"/>
-      <c r="AMG6" s="0"/>
-      <c r="AMH6" s="0"/>
-      <c r="AMI6" s="0"/>
-      <c r="AMJ6" s="0"/>
-    </row>
-    <row r="7" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="AMB6" s="1"/>
+      <c r="AMC6" s="1"/>
+      <c r="AMD6" s="1"/>
+      <c r="AME6" s="1"/>
+      <c r="AMF6" s="1"/>
+      <c r="AMG6" s="1"/>
+      <c r="AMH6" s="1"/>
+      <c r="AMI6" s="1"/>
+      <c r="AMJ6" s="1"/>
+    </row>
+    <row r="7" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="AMB7" s="0"/>
-      <c r="AMC7" s="0"/>
-      <c r="AMD7" s="0"/>
-      <c r="AME7" s="0"/>
-      <c r="AMF7" s="0"/>
-      <c r="AMG7" s="0"/>
-      <c r="AMH7" s="0"/>
-      <c r="AMI7" s="0"/>
-      <c r="AMJ7" s="0"/>
-    </row>
-    <row r="8" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="AMB7" s="1"/>
+      <c r="AMC7" s="1"/>
+      <c r="AMD7" s="1"/>
+      <c r="AME7" s="1"/>
+      <c r="AMF7" s="1"/>
+      <c r="AMG7" s="1"/>
+      <c r="AMH7" s="1"/>
+      <c r="AMI7" s="1"/>
+      <c r="AMJ7" s="1"/>
+    </row>
+    <row r="8" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AMB8" s="0"/>
-      <c r="AMC8" s="0"/>
-      <c r="AMD8" s="0"/>
-      <c r="AME8" s="0"/>
-      <c r="AMF8" s="0"/>
-      <c r="AMG8" s="0"/>
-      <c r="AMH8" s="0"/>
-      <c r="AMI8" s="0"/>
-      <c r="AMJ8" s="0"/>
-    </row>
-    <row r="9" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="AMB8" s="1"/>
+      <c r="AMC8" s="1"/>
+      <c r="AMD8" s="1"/>
+      <c r="AME8" s="1"/>
+      <c r="AMF8" s="1"/>
+      <c r="AMG8" s="1"/>
+      <c r="AMH8" s="1"/>
+      <c r="AMI8" s="1"/>
+      <c r="AMJ8" s="1"/>
+    </row>
+    <row r="9" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="AMB9" s="0"/>
-      <c r="AMC9" s="0"/>
-      <c r="AMD9" s="0"/>
-      <c r="AME9" s="0"/>
-      <c r="AMF9" s="0"/>
-      <c r="AMG9" s="0"/>
-      <c r="AMH9" s="0"/>
-      <c r="AMI9" s="0"/>
-      <c r="AMJ9" s="0"/>
-    </row>
-    <row r="10" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="AMB9" s="1"/>
+      <c r="AMC9" s="1"/>
+      <c r="AMD9" s="1"/>
+      <c r="AME9" s="1"/>
+      <c r="AMF9" s="1"/>
+      <c r="AMG9" s="1"/>
+      <c r="AMH9" s="1"/>
+      <c r="AMI9" s="1"/>
+      <c r="AMJ9" s="1"/>
+    </row>
+    <row r="10" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="AMB10" s="0"/>
-      <c r="AMC10" s="0"/>
-      <c r="AMD10" s="0"/>
-      <c r="AME10" s="0"/>
-      <c r="AMF10" s="0"/>
-      <c r="AMG10" s="0"/>
-      <c r="AMH10" s="0"/>
-      <c r="AMI10" s="0"/>
-      <c r="AMJ10" s="0"/>
-    </row>
-    <row r="11" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="AMB10" s="1"/>
+      <c r="AMC10" s="1"/>
+      <c r="AMD10" s="1"/>
+      <c r="AME10" s="1"/>
+      <c r="AMF10" s="1"/>
+      <c r="AMG10" s="1"/>
+      <c r="AMH10" s="1"/>
+      <c r="AMI10" s="1"/>
+      <c r="AMJ10" s="1"/>
+    </row>
+    <row r="11" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="AMB11" s="0"/>
-      <c r="AMC11" s="0"/>
-      <c r="AMD11" s="0"/>
-      <c r="AME11" s="0"/>
-      <c r="AMF11" s="0"/>
-      <c r="AMG11" s="0"/>
-      <c r="AMH11" s="0"/>
-      <c r="AMI11" s="0"/>
-      <c r="AMJ11" s="0"/>
+        <v>21</v>
+      </c>
+      <c r="AMB11" s="1"/>
+      <c r="AMC11" s="1"/>
+      <c r="AMD11" s="1"/>
+      <c r="AME11" s="1"/>
+      <c r="AMF11" s="1"/>
+      <c r="AMG11" s="1"/>
+      <c r="AMH11" s="1"/>
+      <c r="AMI11" s="1"/>
+      <c r="AMJ11" s="1"/>
     </row>
     <row r="12" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="AMB12" s="0"/>
-      <c r="AMC12" s="0"/>
-      <c r="AMD12" s="0"/>
-      <c r="AME12" s="0"/>
-      <c r="AMF12" s="0"/>
-      <c r="AMG12" s="0"/>
-      <c r="AMH12" s="0"/>
-      <c r="AMI12" s="0"/>
-      <c r="AMJ12" s="0"/>
-    </row>
-    <row r="13" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="AMB12" s="1"/>
+      <c r="AMC12" s="1"/>
+      <c r="AMD12" s="1"/>
+      <c r="AME12" s="1"/>
+      <c r="AMF12" s="1"/>
+      <c r="AMG12" s="1"/>
+      <c r="AMH12" s="1"/>
+      <c r="AMI12" s="1"/>
+      <c r="AMJ12" s="1"/>
+    </row>
+    <row r="13" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="AMB13" s="0"/>
-      <c r="AMC13" s="0"/>
-      <c r="AMD13" s="0"/>
-      <c r="AME13" s="0"/>
-      <c r="AMF13" s="0"/>
-      <c r="AMG13" s="0"/>
-      <c r="AMH13" s="0"/>
-      <c r="AMI13" s="0"/>
-      <c r="AMJ13" s="0"/>
-    </row>
-    <row r="14" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="AMB14" s="0"/>
-      <c r="AMC14" s="0"/>
-      <c r="AMD14" s="0"/>
-      <c r="AME14" s="0"/>
-      <c r="AMF14" s="0"/>
-      <c r="AMG14" s="0"/>
-      <c r="AMH14" s="0"/>
-      <c r="AMI14" s="0"/>
-      <c r="AMJ14" s="0"/>
-    </row>
-    <row r="15" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="AMB13" s="1"/>
+      <c r="AMC13" s="1"/>
+      <c r="AMD13" s="1"/>
+      <c r="AME13" s="1"/>
+      <c r="AMF13" s="1"/>
+      <c r="AMG13" s="1"/>
+      <c r="AMH13" s="1"/>
+      <c r="AMI13" s="1"/>
+      <c r="AMJ13" s="1"/>
+    </row>
+    <row r="14" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AMB15" s="0"/>
-      <c r="AMC15" s="0"/>
-      <c r="AMD15" s="0"/>
-      <c r="AME15" s="0"/>
-      <c r="AMF15" s="0"/>
-      <c r="AMG15" s="0"/>
-      <c r="AMH15" s="0"/>
-      <c r="AMI15" s="0"/>
-      <c r="AMJ15" s="0"/>
-    </row>
-    <row r="16" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+      <c r="AMB14" s="1"/>
+      <c r="AMC14" s="1"/>
+      <c r="AMD14" s="1"/>
+      <c r="AME14" s="1"/>
+      <c r="AMF14" s="1"/>
+      <c r="AMG14" s="1"/>
+      <c r="AMH14" s="1"/>
+      <c r="AMI14" s="1"/>
+      <c r="AMJ14" s="1"/>
+    </row>
+    <row r="15" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="AMB16" s="0"/>
-      <c r="AMC16" s="0"/>
-      <c r="AMD16" s="0"/>
-      <c r="AME16" s="0"/>
-      <c r="AMF16" s="0"/>
-      <c r="AMG16" s="0"/>
-      <c r="AMH16" s="0"/>
-      <c r="AMI16" s="0"/>
-      <c r="AMJ16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="B15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AMB15" s="1"/>
+      <c r="AMC15" s="1"/>
+      <c r="AMD15" s="1"/>
+      <c r="AME15" s="1"/>
+      <c r="AMF15" s="1"/>
+      <c r="AMG15" s="1"/>
+      <c r="AMH15" s="1"/>
+      <c r="AMI15" s="1"/>
+      <c r="AMJ15" s="1"/>
+    </row>
+    <row r="16" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="AMB16" s="1"/>
+      <c r="AMC16" s="1"/>
+      <c r="AMD16" s="1"/>
+      <c r="AME16" s="1"/>
+      <c r="AMF16" s="1"/>
+      <c r="AMG16" s="1"/>
+      <c r="AMH16" s="1"/>
+      <c r="AMI16" s="1"/>
+      <c r="AMJ16" s="1"/>
+    </row>
+    <row r="17" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="B17" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
+      <c r="AMB17" s="1"/>
+      <c r="AMC17" s="1"/>
+      <c r="AMD17" s="1"/>
+      <c r="AME17" s="1"/>
+      <c r="AMF17" s="1"/>
+      <c r="AMG17" s="1"/>
+      <c r="AMH17" s="1"/>
+      <c r="AMI17" s="1"/>
+      <c r="AMJ17" s="1"/>
+    </row>
+    <row r="18" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="AMB18" s="0"/>
-      <c r="AMC18" s="0"/>
-      <c r="AMD18" s="0"/>
-      <c r="AME18" s="0"/>
-      <c r="AMF18" s="0"/>
-      <c r="AMG18" s="0"/>
-      <c r="AMH18" s="0"/>
-      <c r="AMI18" s="0"/>
-      <c r="AMJ18" s="0"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="AMB18" s="1"/>
+      <c r="AMC18" s="1"/>
+      <c r="AMD18" s="1"/>
+      <c r="AME18" s="1"/>
+      <c r="AMF18" s="1"/>
+      <c r="AMG18" s="1"/>
+      <c r="AMH18" s="1"/>
+      <c r="AMI18" s="1"/>
+      <c r="AMJ18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="0" t="s">
+    </row>
+    <row r="20" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="AMB20" s="1"/>
+      <c r="AMC20" s="1"/>
+      <c r="AMD20" s="1"/>
+      <c r="AME20" s="1"/>
+      <c r="AMF20" s="1"/>
+      <c r="AMG20" s="1"/>
+      <c r="AMH20" s="1"/>
+      <c r="AMI20" s="1"/>
+      <c r="AMJ20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="AMB21" s="0"/>
-      <c r="AMC21" s="0"/>
-      <c r="AMD21" s="0"/>
-      <c r="AME21" s="0"/>
-      <c r="AMF21" s="0"/>
-      <c r="AMG21" s="0"/>
-      <c r="AMH21" s="0"/>
-      <c r="AMI21" s="0"/>
-      <c r="AMJ21" s="0"/>
+      <c r="B21" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="B22" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="23" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="AMB23" s="1"/>
+      <c r="AMC23" s="1"/>
+      <c r="AMD23" s="1"/>
+      <c r="AME23" s="1"/>
+      <c r="AMF23" s="1"/>
+      <c r="AMG23" s="1"/>
+      <c r="AMH23" s="1"/>
+      <c r="AMI23" s="1"/>
+      <c r="AMJ23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="C24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" s="0" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="C25" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="AMB27" s="0"/>
-      <c r="AMC27" s="0"/>
-      <c r="AMD27" s="0"/>
-      <c r="AME27" s="0"/>
-      <c r="AMF27" s="0"/>
-      <c r="AMG27" s="0"/>
-      <c r="AMH27" s="0"/>
-      <c r="AMI27" s="0"/>
-      <c r="AMJ27" s="0"/>
-    </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="0" t="s">
+    </row>
+    <row r="29" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
         <v>53</v>
       </c>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="AMB29" s="1"/>
+      <c r="AMC29" s="1"/>
+      <c r="AMD29" s="1"/>
+      <c r="AME29" s="1"/>
+      <c r="AMF29" s="1"/>
+      <c r="AMG29" s="1"/>
+      <c r="AMH29" s="1"/>
+      <c r="AMI29" s="1"/>
+      <c r="AMJ29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="32" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="AMB32" s="0"/>
-      <c r="AMC32" s="0"/>
-      <c r="AMD32" s="0"/>
-      <c r="AME32" s="0"/>
-      <c r="AMF32" s="0"/>
-      <c r="AMG32" s="0"/>
-      <c r="AMH32" s="0"/>
-      <c r="AMI32" s="0"/>
-      <c r="AMJ32" s="0"/>
+      <c r="B32" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="0" t="s">
-        <v>61</v>
+    </row>
+    <row r="34" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="AMB34" s="1"/>
+      <c r="AMC34" s="1"/>
+      <c r="AMD34" s="1"/>
+      <c r="AME34" s="1"/>
+      <c r="AMF34" s="1"/>
+      <c r="AMG34" s="1"/>
+      <c r="AMH34" s="1"/>
+      <c r="AMI34" s="1"/>
+      <c r="AMJ34" s="1"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="6"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="6"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" s="6"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A12:C12"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A44:C44"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B46" r:id="rId1" display="Mohab.Mohie@incorta.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -963,32 +1160,32 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="5" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="7" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>62</v>
+      <c r="A1" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>63</v>
+      <c r="A2" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>64</v>
+      <c r="A3" s="7" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>65</v>
+      <c r="A4" s="7" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>66</v>
+      <c r="A5" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating test data and SHAFT_Engine
. fixing issue with clicking seemingly non-clickable elements
. fixing issue with scheduler date being in the past
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/certification/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/certification/TestData.xlsx
@@ -236,7 +236,7 @@
     <t xml:space="preserve">SchemaLoadJobDate</t>
   </si>
   <si>
-    <t xml:space="preserve">03/20/2018</t>
+    <t xml:space="preserve">12/31/2020</t>
   </si>
   <si>
     <t xml:space="preserve">SchemaLoadJobTime</t>
@@ -404,27 +404,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -440,7 +440,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -521,8 +521,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B41" activeCellId="0" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
minor fixes and test data update
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/certification/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/certification/TestData.xlsx
@@ -113,7 +113,7 @@
     <t xml:space="preserve">IncortaVersion</t>
   </si>
   <si>
-    <t xml:space="preserve">sqli_spark</t>
+    <t xml:space="preserve">master</t>
   </si>
   <si>
     <t xml:space="preserve">TC004 - Add Roles To Group</t>
@@ -522,7 +522,7 @@
   <dimension ref="A1:AMJ46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Including Aggregated Tables Data Validation Support
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/certification/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/certification/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="97">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -32,6 +32,12 @@
     <t xml:space="preserve">Data2</t>
   </si>
   <si>
+    <t xml:space="preserve">Data3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data4</t>
+  </si>
+  <si>
     <t xml:space="preserve">URLs</t>
   </si>
   <si>
@@ -248,7 +254,37 @@
     <t xml:space="preserve">No Recurrence</t>
   </si>
   <si>
-    <t xml:space="preserve">TC016 - Send Dashboard via email</t>
+    <t xml:space="preserve">TC017 - Validate Insight Data (Aggregated Table)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InsightDataRows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InsightDataMeasures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC018 - Send Dashboard via email</t>
   </si>
   <si>
     <t xml:space="preserve">EmailFormat</t>
@@ -512,8 +548,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -534,6 +570,12 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="AMB1" s="3"/>
       <c r="AMC1" s="3"/>
       <c r="AMD1" s="3"/>
@@ -546,7 +588,7 @@
     </row>
     <row r="2" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -562,10 +604,10 @@
     </row>
     <row r="3" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AMB3" s="1"/>
       <c r="AMC3" s="1"/>
@@ -579,10 +621,10 @@
     </row>
     <row r="4" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AMB4" s="1"/>
       <c r="AMC4" s="1"/>
@@ -596,10 +638,10 @@
     </row>
     <row r="5" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="AMB5" s="1"/>
       <c r="AMC5" s="1"/>
@@ -613,10 +655,10 @@
     </row>
     <row r="6" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AMB6" s="1"/>
       <c r="AMC6" s="1"/>
@@ -630,10 +672,10 @@
     </row>
     <row r="7" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="AMB7" s="1"/>
       <c r="AMC7" s="1"/>
@@ -647,10 +689,10 @@
     </row>
     <row r="8" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AMB8" s="1"/>
       <c r="AMC8" s="1"/>
@@ -664,10 +706,10 @@
     </row>
     <row r="9" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AMB9" s="1"/>
       <c r="AMC9" s="1"/>
@@ -681,10 +723,10 @@
     </row>
     <row r="10" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="AMB10" s="1"/>
       <c r="AMC10" s="1"/>
@@ -698,10 +740,10 @@
     </row>
     <row r="11" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="AMB11" s="1"/>
       <c r="AMC11" s="1"/>
@@ -715,7 +757,7 @@
     </row>
     <row r="12" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -731,10 +773,10 @@
     </row>
     <row r="13" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="AMB13" s="1"/>
       <c r="AMC13" s="1"/>
@@ -748,10 +790,10 @@
     </row>
     <row r="14" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AMB14" s="1"/>
       <c r="AMC14" s="1"/>
@@ -765,10 +807,10 @@
     </row>
     <row r="15" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AMB15" s="1"/>
       <c r="AMC15" s="1"/>
@@ -782,7 +824,7 @@
     </row>
     <row r="16" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -798,18 +840,18 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -825,23 +867,23 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -857,40 +899,40 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="C24" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>30</v>
@@ -901,18 +943,18 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -928,39 +970,39 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -976,112 +1018,179 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
+      <c r="AMB35" s="1"/>
+      <c r="AMC35" s="1"/>
+      <c r="AMD35" s="1"/>
+      <c r="AME35" s="1"/>
+      <c r="AMF35" s="1"/>
+      <c r="AMG35" s="1"/>
+      <c r="AMH35" s="1"/>
+      <c r="AMI35" s="1"/>
+      <c r="AMJ35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C37" s="6"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C38" s="6"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C39" s="6"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C40" s="6"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C41" s="6"/>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
+      <c r="AMB42" s="1"/>
+      <c r="AMC42" s="1"/>
+      <c r="AMD42" s="1"/>
+      <c r="AME42" s="1"/>
+      <c r="AMF42" s="1"/>
+      <c r="AMG42" s="1"/>
+      <c r="AMH42" s="1"/>
+      <c r="AMI42" s="1"/>
+      <c r="AMJ42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C43" s="6"/>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>79</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>84</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="AMB45" s="1"/>
+      <c r="AMC45" s="1"/>
+      <c r="AMD45" s="1"/>
+      <c r="AME45" s="1"/>
+      <c r="AMF45" s="1"/>
+      <c r="AMG45" s="1"/>
+      <c r="AMH45" s="1"/>
+      <c r="AMI45" s="1"/>
+      <c r="AMJ45" s="1"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A16:C16"/>
@@ -1091,9 +1200,10 @@
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A45:C45"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B44" r:id="rId1" display="Mohab.Mohie@incorta.com"/>
+    <hyperlink ref="B47" r:id="rId1" display="Mohab.Mohie@incorta.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1124,27 +1234,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
attempting certification path test data fix + engine upgrade
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/certification/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/certification/TestData.xlsx
@@ -281,7 +281,7 @@
     <t xml:space="preserve">90</t>
   </si>
   <si>
-    <t xml:space="preserve">120</t>
+    <t xml:space="preserve">75</t>
   </si>
   <si>
     <t xml:space="preserve">TC018 - Send Dashboard via email</t>
@@ -532,8 +532,8 @@
   </sheetPr>
   <dimension ref="A1:Z48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B46" activeCellId="0" sqref="B46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D44" activeCellId="0" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3210,7 +3210,6 @@
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>